<commit_message>
Updated experiment + added answers
</commit_message>
<xml_diff>
--- a/lab5/shortTimingExperiment.xlsx
+++ b/lab5/shortTimingExperiment.xlsx
@@ -756,7 +756,7 @@
                   <c:v>12.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>67.87</c:v>
+                  <c:v>49.95</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>203.04</c:v>
@@ -774,11 +774,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164449280"/>
-        <c:axId val="164447744"/>
+        <c:axId val="146739968"/>
+        <c:axId val="146741888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164449280"/>
+        <c:axId val="146739968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -809,13 +809,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164447744"/>
+        <c:crossAx val="146741888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164447744"/>
+        <c:axId val="146741888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="210"/>
@@ -852,7 +852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164449280"/>
+        <c:crossAx val="146739968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="30"/>
@@ -1200,7 +1200,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
         <v>1.7495703605200001E-4</v>
       </c>
       <c r="C7">
-        <v>67.87</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>